<commit_message>
Updated dataset to include final week of sampling.
</commit_message>
<xml_diff>
--- a/Data/Season2/Encounters - Double observer - no distance (Responses).xlsx
+++ b/Data/Season2/Encounters - Double observer - no distance (Responses).xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="37">
   <si>
     <t>Timestamp</t>
   </si>
@@ -132,6 +132,12 @@
   <si>
     <t xml:space="preserve">Horrible visibility! </t>
   </si>
+  <si>
+    <t>Shellfish, Broken shell</t>
+  </si>
+  <si>
+    <t>Roots</t>
+  </si>
 </sst>
 </file>
 
@@ -7204,6 +7210,2345 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="233">
+      <c r="A233" s="2">
+        <v>43334.70626708333</v>
+      </c>
+      <c r="B233" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E233" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="F233" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="G233" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H233" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="I233" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J233" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="2">
+        <v>43334.706593194445</v>
+      </c>
+      <c r="B234" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E234" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="F234" s="1">
+        <v>11.71</v>
+      </c>
+      <c r="G234" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H234" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I234" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J234" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="2">
+        <v>43334.70688079861</v>
+      </c>
+      <c r="B235" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E235" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F235" s="1">
+        <v>11.54</v>
+      </c>
+      <c r="G235" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H235" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="I235" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J235" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="2">
+        <v>43334.707152800926</v>
+      </c>
+      <c r="B236" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E236" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F236" s="1">
+        <v>12.13</v>
+      </c>
+      <c r="G236" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H236" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="I236" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J236" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="2">
+        <v>43334.70798390046</v>
+      </c>
+      <c r="B237" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E237" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F237" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="G237" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H237" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="I237" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J237" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="2">
+        <v>43334.70822326389</v>
+      </c>
+      <c r="B238" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E238" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F238" s="1">
+        <v>13.2</v>
+      </c>
+      <c r="G238" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H238" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="I238" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J238" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="2">
+        <v>43334.70843925926</v>
+      </c>
+      <c r="B239" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E239" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F239" s="1">
+        <v>12.68</v>
+      </c>
+      <c r="G239" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H239" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="I239" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J239" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="2">
+        <v>43334.70872314815</v>
+      </c>
+      <c r="B240" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E240" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F240" s="1">
+        <v>13.54</v>
+      </c>
+      <c r="G240" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H240" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="I240" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J240" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="2">
+        <v>43334.70893356482</v>
+      </c>
+      <c r="B241" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E241" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F241" s="1">
+        <v>13.85</v>
+      </c>
+      <c r="G241" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H241" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="I241" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J241" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="2">
+        <v>43334.70915740741</v>
+      </c>
+      <c r="B242" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E242" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F242" s="1">
+        <v>13.9</v>
+      </c>
+      <c r="G242" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H242" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="I242" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J242" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="2">
+        <v>43334.70937502314</v>
+      </c>
+      <c r="B243" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E243" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F243" s="1">
+        <v>14.27</v>
+      </c>
+      <c r="G243" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H243" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="I243" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="J243" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="2">
+        <v>43334.70972309027</v>
+      </c>
+      <c r="B244" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E244" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F244" s="1">
+        <v>14.71</v>
+      </c>
+      <c r="G244" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H244" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I244" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J244" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="2">
+        <v>43334.71002059028</v>
+      </c>
+      <c r="B245" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E245" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F245" s="1">
+        <v>14.95</v>
+      </c>
+      <c r="G245" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="H245" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="I245" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J245" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="2">
+        <v>43334.7102297338</v>
+      </c>
+      <c r="B246" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E246" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F246" s="1">
+        <v>15.08</v>
+      </c>
+      <c r="G246" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H246" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I246" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J246" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="2">
+        <v>43334.71044703704</v>
+      </c>
+      <c r="B247" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E247" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F247" s="1">
+        <v>15.04</v>
+      </c>
+      <c r="G247" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H247" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="I247" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J247" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="2">
+        <v>43334.710799803244</v>
+      </c>
+      <c r="B248" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E248" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F248" s="1">
+        <v>15.23</v>
+      </c>
+      <c r="G248" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H248" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="I248" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J248" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="2">
+        <v>43334.710994953704</v>
+      </c>
+      <c r="B249" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E249" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F249" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="G249" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H249" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I249" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J249" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="2">
+        <v>43334.711210208334</v>
+      </c>
+      <c r="B250" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E250" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F250" s="1">
+        <v>16.96</v>
+      </c>
+      <c r="G250" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H250" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="I250" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="J250" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="2">
+        <v>43334.71150949074</v>
+      </c>
+      <c r="B251" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E251" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F251" s="1">
+        <v>16.97</v>
+      </c>
+      <c r="G251" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H251" s="1">
+        <v>2.2</v>
+      </c>
+      <c r="I251" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J251" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="2">
+        <v>43334.711789733796</v>
+      </c>
+      <c r="B252" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E252" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F252" s="1">
+        <v>17.65</v>
+      </c>
+      <c r="G252" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H252" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="I252" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J252" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="2">
+        <v>43334.71203011574</v>
+      </c>
+      <c r="B253" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E253" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F253" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="G253" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H253" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="I253" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J253" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="2">
+        <v>43334.715225023145</v>
+      </c>
+      <c r="B254" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E254" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F254" s="1">
+        <v>18.11</v>
+      </c>
+      <c r="G254" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H254" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I254" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J254" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="2">
+        <v>43334.71582898148</v>
+      </c>
+      <c r="B255" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E255" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F255" s="1">
+        <v>18.34</v>
+      </c>
+      <c r="G255" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H255" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I255" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J255" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="2">
+        <v>43334.71610883102</v>
+      </c>
+      <c r="B256" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E256" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F256" s="1">
+        <v>13.19</v>
+      </c>
+      <c r="G256" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H256" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I256" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J256" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="2">
+        <v>43334.716384259256</v>
+      </c>
+      <c r="B257" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E257" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F257" s="1">
+        <v>17.28</v>
+      </c>
+      <c r="G257" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="H257" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="I257" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="J257" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="2">
+        <v>43334.71663137732</v>
+      </c>
+      <c r="B258" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E258" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F258" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="G258" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H258" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="I258" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J258" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="2">
+        <v>43334.71705262731</v>
+      </c>
+      <c r="B259" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E259" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F259" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="G259" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H259" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="I259" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J259" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="2">
+        <v>43334.717442546294</v>
+      </c>
+      <c r="B260" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E260" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F260" s="1">
+        <v>5.95</v>
+      </c>
+      <c r="G260" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H260" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="I260" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J260" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="2">
+        <v>43334.7177059838</v>
+      </c>
+      <c r="B261" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E261" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F261" s="1">
+        <v>5.9</v>
+      </c>
+      <c r="G261" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H261" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="I261" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="J261" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="2">
+        <v>43334.71813483797</v>
+      </c>
+      <c r="B262" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E262" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F262" s="1">
+        <v>6.54</v>
+      </c>
+      <c r="G262" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H262" s="1">
+        <v>1.1</v>
+      </c>
+      <c r="I262" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J262" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="2">
+        <v>43334.7187212037</v>
+      </c>
+      <c r="B263" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E263" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F263" s="1">
+        <v>6.93</v>
+      </c>
+      <c r="G263" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H263" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="I263" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J263" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="2">
+        <v>43334.71897777778</v>
+      </c>
+      <c r="B264" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E264" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F264" s="1">
+        <v>7.32</v>
+      </c>
+      <c r="G264" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H264" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="I264" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J264" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="2">
+        <v>43334.71919268518</v>
+      </c>
+      <c r="B265" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E265" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F265" s="1">
+        <v>7.64</v>
+      </c>
+      <c r="G265" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H265" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="I265" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J265" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="2">
+        <v>43334.71938405093</v>
+      </c>
+      <c r="B266" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E266" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F266" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G266" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H266" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I266" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J266" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="2">
+        <v>43334.71961252315</v>
+      </c>
+      <c r="B267" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E267" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F267" s="1">
+        <v>8.83</v>
+      </c>
+      <c r="G267" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H267" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="I267" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="J267" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="2">
+        <v>43334.71979663194</v>
+      </c>
+      <c r="B268" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E268" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F268" s="1">
+        <v>9.49</v>
+      </c>
+      <c r="G268" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H268" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="I268" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J268" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="2">
+        <v>43334.72002337963</v>
+      </c>
+      <c r="B269" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E269" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F269" s="1">
+        <v>9.53</v>
+      </c>
+      <c r="G269" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H269" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="I269" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J269" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="2">
+        <v>43334.720246620374</v>
+      </c>
+      <c r="B270" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E270" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F270" s="1">
+        <v>9.56</v>
+      </c>
+      <c r="G270" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H270" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="I270" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J270" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="2">
+        <v>43334.72043295139</v>
+      </c>
+      <c r="B271" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E271" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F271" s="1">
+        <v>10.19</v>
+      </c>
+      <c r="G271" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H271" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I271" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="J271" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="2">
+        <v>43334.720681226856</v>
+      </c>
+      <c r="B272" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E272" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F272" s="1">
+        <v>11.38</v>
+      </c>
+      <c r="G272" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H272" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="I272" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="J272" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="2">
+        <v>43334.721053472225</v>
+      </c>
+      <c r="B273" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E273" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F273" s="1">
+        <v>11.8</v>
+      </c>
+      <c r="G273" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H273" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I273" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="J273" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="2">
+        <v>43334.721279618054</v>
+      </c>
+      <c r="B274" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E274" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F274" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G274" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H274" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="I274" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J274" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="2">
+        <v>43334.72148756945</v>
+      </c>
+      <c r="B275" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E275" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F275" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="G275" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H275" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="I275" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J275" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="2">
+        <v>43334.72171373843</v>
+      </c>
+      <c r="B276" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E276" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F276" s="1">
+        <v>10.03</v>
+      </c>
+      <c r="G276" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H276" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I276" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J276" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="2">
+        <v>43334.72188981481</v>
+      </c>
+      <c r="B277" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E277" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F277" s="1">
+        <v>10.07</v>
+      </c>
+      <c r="G277" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H277" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="I277" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J277" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="2">
+        <v>43334.72209377315</v>
+      </c>
+      <c r="B278" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E278" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F278" s="1">
+        <v>10.09</v>
+      </c>
+      <c r="G278" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H278" s="1">
+        <v>1.1</v>
+      </c>
+      <c r="I278" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J278" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="2">
+        <v>43334.72236347222</v>
+      </c>
+      <c r="B279" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E279" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F279" s="1">
+        <v>10.21</v>
+      </c>
+      <c r="G279" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H279" s="1">
+        <v>2.3</v>
+      </c>
+      <c r="I279" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="J279" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="2">
+        <v>43334.72257521991</v>
+      </c>
+      <c r="B280" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E280" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F280" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="G280" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H280" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I280" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="J280" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="2">
+        <v>43334.72274520833</v>
+      </c>
+      <c r="B281" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E281" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F281" s="1">
+        <v>2.77</v>
+      </c>
+      <c r="G281" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H281" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I281" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J281" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="2">
+        <v>43334.722962789354</v>
+      </c>
+      <c r="B282" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E282" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F282" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G282" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H282" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I282" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J282" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="2">
+        <v>43334.723204131944</v>
+      </c>
+      <c r="B283" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E283" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F283" s="1">
+        <v>5.95</v>
+      </c>
+      <c r="G283" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H283" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I283" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="J283" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="2">
+        <v>43334.723390520834</v>
+      </c>
+      <c r="B284" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E284" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F284" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="G284" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H284" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I284" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J284" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="2">
+        <v>43334.72363896991</v>
+      </c>
+      <c r="B285" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E285" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F285" s="1">
+        <v>7.49</v>
+      </c>
+      <c r="G285" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H285" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="I285" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J285" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="2">
+        <v>43334.72382925926</v>
+      </c>
+      <c r="B286" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E286" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F286" s="1">
+        <v>7.53</v>
+      </c>
+      <c r="G286" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H286" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="I286" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J286" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="2">
+        <v>43334.72402253472</v>
+      </c>
+      <c r="B287" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E287" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F287" s="1">
+        <v>8.28</v>
+      </c>
+      <c r="G287" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H287" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="I287" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="J287" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="2">
+        <v>43334.724200833334</v>
+      </c>
+      <c r="B288" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E288" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F288" s="1">
+        <v>9.27</v>
+      </c>
+      <c r="G288" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H288" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="I288" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J288" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="2">
+        <v>43334.724371331016</v>
+      </c>
+      <c r="B289" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E289" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F289" s="1">
+        <v>9.84</v>
+      </c>
+      <c r="G289" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H289" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="I289" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J289" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="2">
+        <v>43334.72462421296</v>
+      </c>
+      <c r="B290" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E290" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F290" s="1">
+        <v>9.69</v>
+      </c>
+      <c r="G290" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="H290" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I290" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J290" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="2">
+        <v>43334.7851028125</v>
+      </c>
+      <c r="B291" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E291" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F291" s="1">
+        <v>11.13</v>
+      </c>
+      <c r="G291" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H291" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="I291" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J291" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="2">
+        <v>43334.7854421875</v>
+      </c>
+      <c r="B292" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E292" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F292" s="1">
+        <v>12.86</v>
+      </c>
+      <c r="G292" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="H292" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I292" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J292" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="2">
+        <v>43334.785694108796</v>
+      </c>
+      <c r="B293" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E293" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F293" s="1">
+        <v>14.7</v>
+      </c>
+      <c r="G293" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H293" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I293" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="J293" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="2">
+        <v>43334.78636197917</v>
+      </c>
+      <c r="B294" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E294" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F294" s="1">
+        <v>14.71</v>
+      </c>
+      <c r="G294" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H294" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I294" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J294" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="2">
+        <v>43334.78667598379</v>
+      </c>
+      <c r="B295" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D295" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E295" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F295" s="1">
+        <v>15.92</v>
+      </c>
+      <c r="G295" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H295" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="I295" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J295" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="2">
+        <v>43334.78699494213</v>
+      </c>
+      <c r="B296" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D296" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E296" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F296" s="1">
+        <v>0.28</v>
+      </c>
+      <c r="G296" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H296" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="I296" s="1">
+        <v>2.2</v>
+      </c>
+      <c r="J296" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="2">
+        <v>43334.787276689814</v>
+      </c>
+      <c r="B297" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D297" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E297" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F297" s="1">
+        <v>1.56</v>
+      </c>
+      <c r="G297" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="H297" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="I297" s="1">
+        <v>9.8</v>
+      </c>
+      <c r="J297" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="2">
+        <v>43334.787501493054</v>
+      </c>
+      <c r="B298" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D298" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E298" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F298" s="1">
+        <v>3.29</v>
+      </c>
+      <c r="G298" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H298" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I298" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J298" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="2">
+        <v>43334.78778983797</v>
+      </c>
+      <c r="B299" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D299" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E299" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F299" s="1">
+        <v>4.06</v>
+      </c>
+      <c r="G299" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H299" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I299" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="J299" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="2">
+        <v>43334.788065138884</v>
+      </c>
+      <c r="B300" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D300" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E300" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F300" s="1">
+        <v>4.51</v>
+      </c>
+      <c r="G300" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H300" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="I300" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J300" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="2">
+        <v>43334.788287731484</v>
+      </c>
+      <c r="B301" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D301" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E301" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F301" s="1">
+        <v>6.31</v>
+      </c>
+      <c r="G301" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H301" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="I301" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J301" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="2">
+        <v>43334.78872303241</v>
+      </c>
+      <c r="B302" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D302" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E302" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F302" s="1">
+        <v>9.8</v>
+      </c>
+      <c r="G302" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H302" s="1">
+        <v>4.1</v>
+      </c>
+      <c r="I302" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J302" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K302" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="2">
+        <v>43334.78948039352</v>
+      </c>
+      <c r="B303" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D303" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E303" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F303" s="1">
+        <v>14.35</v>
+      </c>
+      <c r="G303" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H303" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="I303" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="J303" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="2">
+        <v>43334.79047317129</v>
+      </c>
+      <c r="B304" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E304" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F304" s="1">
+        <v>17.82</v>
+      </c>
+      <c r="G304" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H304" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="I304" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J304" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="2">
+        <v>43334.790778842595</v>
+      </c>
+      <c r="B305" s="3">
+        <v>43333.0</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E305" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F305" s="1">
+        <v>18.8</v>
+      </c>
+      <c r="G305" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="H305" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="I305" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="J305" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>